<commit_message>
Update para DBs vazios
</commit_message>
<xml_diff>
--- a/db_apostas.xlsx
+++ b/db_apostas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programação\Python\Projetos\Dashboard Apostas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266BCEA2-732C-4818-83FC-49EDECB1841F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A5B01E-E268-4A76-8725-3245D45310E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:I403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implementação da opção crédito de apostas
</commit_message>
<xml_diff>
--- a/db_apostas.xlsx
+++ b/db_apostas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programação\Python\Projetos\Dashboard Apostas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30894D20-33FD-46EF-962D-B2401E3C6BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D13EA2E-F491-4655-8B96-3A0016AB286E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Data</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Investimento</t>
+  </si>
+  <si>
+    <t>Crédito de aposta</t>
   </si>
   <si>
     <t>Finalização</t>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I405"/>
+  <dimension ref="A1:J565"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,12 +412,13 @@
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -436,68 +440,71 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -1666,6 +1673,486 @@
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" s="1"/>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="1"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="1"/>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="1"/>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="1"/>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="1"/>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="1"/>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="1"/>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="1"/>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="1"/>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="1"/>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="1"/>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="1"/>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="1"/>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="1"/>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="1"/>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="1"/>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="1"/>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="1"/>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="1"/>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="1"/>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="1"/>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="1"/>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="1"/>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="1"/>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="1"/>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="1"/>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="1"/>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="1"/>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="1"/>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="1"/>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="1"/>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="1"/>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="1"/>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="1"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="1"/>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="1"/>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="1"/>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="1"/>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="1"/>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="1"/>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="1"/>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="1"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="1"/>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="1"/>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="1"/>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="1"/>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="1"/>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="1"/>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="1"/>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="1"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="1"/>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="1"/>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="1"/>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="1"/>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="1"/>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="1"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="1"/>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="1"/>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="1"/>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="1"/>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="1"/>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="1"/>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="1"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="1"/>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="1"/>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="1"/>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="1"/>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="1"/>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="1"/>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="1"/>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="1"/>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="1"/>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="1"/>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="1"/>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="1"/>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="1"/>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="1"/>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="1"/>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="1"/>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="1"/>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="1"/>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="1"/>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="1"/>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="1"/>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="1"/>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="1"/>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="1"/>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="1"/>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="1"/>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="1"/>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="1"/>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="1"/>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="1"/>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="1"/>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="1"/>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="1"/>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="1"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="1"/>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="1"/>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="1"/>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="1"/>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="1"/>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="1"/>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="1"/>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="1"/>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="1"/>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="1"/>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="1"/>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="1"/>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="1"/>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="1"/>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="1"/>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="1"/>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="1"/>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="1"/>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="1"/>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="1"/>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="1"/>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="1"/>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" s="1"/>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" s="1"/>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" s="1"/>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" s="1"/>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" s="1"/>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" s="1"/>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" s="1"/>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" s="1"/>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" s="1"/>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" s="1"/>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" s="1"/>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" s="1"/>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" s="1"/>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" s="1"/>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" s="1"/>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" s="1"/>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" s="1"/>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" s="1"/>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" s="1"/>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" s="1"/>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" s="1"/>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" s="1"/>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" s="1"/>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" s="1"/>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" s="1"/>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" s="1"/>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" s="1"/>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" s="1"/>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" s="1"/>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" s="1"/>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" s="1"/>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" s="1"/>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" s="1"/>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" s="1"/>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" s="1"/>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560" s="1"/>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561" s="1"/>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562" s="1"/>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563" s="1"/>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A564" s="1"/>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A565" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>